<commit_message>
Completed parallel run and Extent Report implementation
</commit_message>
<xml_diff>
--- a/runManager.xlsx
+++ b/runManager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preetammitra/Desktop/Learn EveryDay/Automation Workspaces/All in 1 Workspace/testngUpdated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA198F-0E10-F441-B95A-7768750239A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DECCF1-B5F0-8C4C-91BC-47174EA6FE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -42,31 +42,49 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>validateHotelIsSelected</t>
-  </si>
-  <si>
     <t>validateOfferesIsSelected</t>
   </si>
   <si>
-    <t>validateOfferesIsSelected2</t>
-  </si>
-  <si>
     <t>validateHotelIsSelected2</t>
   </si>
   <si>
+    <t>Testing Link Broken</t>
+  </si>
+  <si>
+    <t>Testing Link Checkboxes</t>
+  </si>
+  <si>
+    <t>Testing Link Checkboxes Negative</t>
+  </si>
+  <si>
+    <t>validateOfferesIsSelectedNegative</t>
+  </si>
+  <si>
+    <t>Testing Link Broken 2</t>
+  </si>
+  <si>
+    <t>validateBrokenIsSelected</t>
+  </si>
+  <si>
+    <t>searchFlights</t>
+  </si>
+  <si>
+    <t>Validating Search resrch result</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Testing Link Broken</t>
-  </si>
-  <si>
-    <t>Testing Link Checkboxes</t>
-  </si>
-  <si>
-    <t>Testing Link Checkboxes Negative</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>searchFlights2</t>
+  </si>
+  <si>
+    <t>searchFlights3</t>
+  </si>
+  <si>
+    <t>searchFlights4</t>
   </si>
 </sst>
 </file>
@@ -399,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -433,30 +451,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -467,13 +485,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -484,24 +502,92 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{3E60C9DF-DB53-4D99-9559-C57CE9C73983}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{3E60C9DF-DB53-4D99-9559-C57CE9C73983}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix after parallel run and multi broswer functionality update
</commit_message>
<xml_diff>
--- a/runManager.xlsx
+++ b/runManager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preetammitra/Desktop/Learn EveryDay/Automation Workspaces/All in 1 Workspace/testngUpdated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DECCF1-B5F0-8C4C-91BC-47174EA6FE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3208DEC-4207-4D40-B000-AB55D0E2EC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added amazon test case
</commit_message>
<xml_diff>
--- a/runManager.xlsx
+++ b/runManager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preetammitra/Desktop/Learn EveryDay/Automation Workspaces/All in 1 Workspace/testngUpdated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3208DEC-4207-4D40-B000-AB55D0E2EC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CECD3A1-05FC-2146-A6D7-865B99C4530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>searchFlights4</t>
+  </si>
+  <si>
+    <t>searchProduct</t>
+  </si>
+  <si>
+    <t>validate the Sorting works</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,7 +531,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -585,9 +591,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{3E60C9DF-DB53-4D99-9559-C57CE9C73983}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{3E60C9DF-DB53-4D99-9559-C57CE9C73983}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
installing chrome in actions 2
</commit_message>
<xml_diff>
--- a/runManager.xlsx
+++ b/runManager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preetammitra/Desktop/Learn EveryDay/IntelliJ/CodeBasse/testNgWithDocker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A498BE-A83E-D940-99D6-E632A2BE40C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13834B0C-8195-464C-841E-290822125A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19900" windowHeight="7540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,7 +615,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -632,7 +632,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>1</v>

</xml_diff>

<commit_message>
Final Commit with github actions changes
</commit_message>
<xml_diff>
--- a/runManager.xlsx
+++ b/runManager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preetammitra/Desktop/Learn EveryDay/IntelliJ/CodeBasse/testNgWithDocker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13834B0C-8195-464C-841E-290822125A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96231F4D-07ED-9242-94C1-FCDDDB5A9235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19900" windowHeight="7540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +133,13 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -161,9 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,7 +548,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
@@ -615,10 +623,10 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -632,10 +640,10 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -652,7 +660,7 @@
         <v>21</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>

</xml_diff>